<commit_message>
Data updates July release part 1
</commit_message>
<xml_diff>
--- a/static/download/2023/RP3_APT_ATC_PRE_2023_Jan_Dec.xlsx
+++ b/static/download/2023/RP3_APT_ATC_PRE_2023_Jan_Dec.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="131">
   <si>
     <t>Data source</t>
   </si>
@@ -396,17 +396,26 @@
   </si>
   <si>
     <t>Comment</t>
+  </si>
+  <si>
+    <t>EDDM, EDDS</t>
+  </si>
+  <si>
+    <t>ATC pre-departure delays added for EDDM and EDDS, All pre-departure delays added for EDDS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Figures updated with additional data (old 31,494 ; 10,577)
+</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <numFmts count="4">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="d&quot; &quot;mmm&quot; &quot;yyyy"/>
     <numFmt numFmtId="165" formatCode="m/d/yyyy"/>
     <numFmt numFmtId="166" formatCode="d mmm yyyy"/>
-    <numFmt numFmtId="167" formatCode="dd-mm-yyyy"/>
   </numFmts>
   <fonts count="12">
     <font>
@@ -539,7 +548,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="35">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -632,9 +641,6 @@
     </xf>
     <xf borderId="0" fillId="3" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="3" fontId="7" numFmtId="167" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="3" fontId="7" numFmtId="17" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment vertical="bottom"/>
@@ -720,7 +726,7 @@
         <v>5</v>
       </c>
       <c r="B2" s="8">
-        <v>45338.0</v>
+        <v>45477.0</v>
       </c>
       <c r="C2" s="9" t="s">
         <v>6</v>
@@ -834,7 +840,7 @@
         <v>1826547.0</v>
       </c>
       <c r="I6" s="24">
-        <f t="shared" ref="I6:I12" si="2">H6/G6</f>
+        <f t="shared" ref="I6:I17" si="2">H6/G6</f>
         <v>19.3001511</v>
       </c>
     </row>
@@ -972,7 +978,7 @@
         <v>11998.0</v>
       </c>
       <c r="F11" s="24">
-        <f>E11/D11</f>
+        <f t="shared" ref="F11:F14" si="3">E11/D11</f>
         <v>0.158804532</v>
       </c>
       <c r="G11" s="23">
@@ -996,9 +1002,16 @@
       <c r="C12" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="D12" s="23"/>
-      <c r="E12" s="23"/>
-      <c r="F12" s="24"/>
+      <c r="D12" s="23">
+        <v>149830.0</v>
+      </c>
+      <c r="E12" s="23">
+        <v>735.0</v>
+      </c>
+      <c r="F12" s="24">
+        <f t="shared" si="3"/>
+        <v>0.004905559634</v>
+      </c>
       <c r="G12" s="23">
         <v>149830.0</v>
       </c>
@@ -1020,12 +1033,26 @@
       <c r="C13" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="D13" s="23"/>
-      <c r="E13" s="23"/>
-      <c r="F13" s="24"/>
-      <c r="G13" s="23"/>
-      <c r="H13" s="23"/>
-      <c r="I13" s="24"/>
+      <c r="D13" s="23">
+        <v>42730.0</v>
+      </c>
+      <c r="E13" s="23">
+        <v>2558.0</v>
+      </c>
+      <c r="F13" s="24">
+        <f t="shared" si="3"/>
+        <v>0.05986426398</v>
+      </c>
+      <c r="G13" s="23">
+        <v>42730.0</v>
+      </c>
+      <c r="H13" s="23">
+        <v>613952.62</v>
+      </c>
+      <c r="I13" s="24">
+        <f t="shared" si="2"/>
+        <v>14.36818675</v>
+      </c>
     </row>
     <row r="14" ht="12.75" customHeight="1">
       <c r="A14" s="21" t="s">
@@ -1044,7 +1071,7 @@
         <v>8364.0</v>
       </c>
       <c r="F14" s="24">
-        <f>E14/D14</f>
+        <f t="shared" si="3"/>
         <v>0.1186517619</v>
       </c>
       <c r="G14" s="23">
@@ -1054,7 +1081,7 @@
         <v>747833.54</v>
       </c>
       <c r="I14" s="24">
-        <f t="shared" ref="I14:I17" si="3">H14/G14</f>
+        <f t="shared" si="2"/>
         <v>10.60877178</v>
       </c>
     </row>
@@ -1078,7 +1105,7 @@
         <v>5448924.46</v>
       </c>
       <c r="I15" s="24">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>24.00904355</v>
       </c>
     </row>
@@ -1102,7 +1129,7 @@
         <v>2472222.0</v>
       </c>
       <c r="I16" s="24">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>20.54074129</v>
       </c>
     </row>
@@ -1133,7 +1160,7 @@
         <v>1793797.59</v>
       </c>
       <c r="I17" s="24">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>15.79269607</v>
       </c>
     </row>
@@ -1409,14 +1436,14 @@
         <v>77</v>
       </c>
       <c r="D28" s="23">
-        <v>31494.0</v>
+        <v>34229.0</v>
       </c>
       <c r="E28" s="23">
-        <v>10577.0</v>
+        <v>11475.0</v>
       </c>
       <c r="F28" s="24">
         <f t="shared" ref="F28:F31" si="6">E28/D28</f>
-        <v>0.3358417476</v>
+        <v>0.3352420462</v>
       </c>
       <c r="G28" s="23">
         <v>31494.0</v>
@@ -1915,14 +1942,14 @@
         <v>118</v>
       </c>
       <c r="D45" s="23">
-        <v>51002.0</v>
+        <v>51003.0</v>
       </c>
       <c r="E45" s="23">
         <v>19041.0</v>
       </c>
       <c r="F45" s="24">
         <f t="shared" si="8"/>
-        <v>0.3733383005</v>
+        <v>0.3733309805</v>
       </c>
       <c r="G45" s="23">
         <v>55800.0</v>
@@ -2013,7 +2040,7 @@
   <sheetFormatPr customHeight="1" defaultColWidth="15.13" defaultRowHeight="15.0"/>
   <cols>
     <col customWidth="1" min="1" max="1" width="11.0"/>
-    <col customWidth="1" min="2" max="2" width="4.38"/>
+    <col customWidth="1" min="2" max="2" width="8.88"/>
     <col customWidth="1" min="3" max="3" width="10.13"/>
     <col customWidth="1" min="4" max="4" width="104.13"/>
   </cols>
@@ -2033,28 +2060,44 @@
       </c>
     </row>
     <row r="2" ht="12.75" customHeight="1">
-      <c r="A2" s="28"/>
-      <c r="B2" s="29"/>
-      <c r="C2" s="30"/>
-      <c r="D2" s="29"/>
-    </row>
-    <row r="3" ht="12.75" customHeight="1">
-      <c r="A3" s="31"/>
-      <c r="B3" s="13"/>
-      <c r="C3" s="13"/>
-      <c r="D3" s="13"/>
+      <c r="A2" s="28">
+        <v>45477.0</v>
+      </c>
+      <c r="B2" s="29" t="s">
+        <v>128</v>
+      </c>
+      <c r="C2" s="30">
+        <v>2023.0</v>
+      </c>
+      <c r="D2" s="29" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="3" ht="14.25" customHeight="1">
+      <c r="A3" s="28">
+        <v>45477.0</v>
+      </c>
+      <c r="B3" s="29" t="s">
+        <v>76</v>
+      </c>
+      <c r="C3" s="30">
+        <v>2023.0</v>
+      </c>
+      <c r="D3" s="29" t="s">
+        <v>130</v>
+      </c>
     </row>
     <row r="4" ht="12.75" customHeight="1">
       <c r="A4" s="28"/>
-      <c r="B4" s="32"/>
-      <c r="C4" s="33"/>
-      <c r="D4" s="34"/>
+      <c r="B4" s="31"/>
+      <c r="C4" s="32"/>
+      <c r="D4" s="33"/>
     </row>
     <row r="5" ht="12.75" customHeight="1">
-      <c r="A5" s="35"/>
-      <c r="B5" s="32"/>
-      <c r="C5" s="33"/>
-      <c r="D5" s="34"/>
+      <c r="A5" s="34"/>
+      <c r="B5" s="31"/>
+      <c r="C5" s="32"/>
+      <c r="D5" s="33"/>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>

</xml_diff>